<commit_message>
Starts Chapter 6 - Adds a subsection on GLMM with R in Chapter 4 - Writes a bit of chapter 6, Experiment 1, up to Analyses section, and renders pdf - As usual, updates in ToC doc and xlsx, and bib file
</commit_message>
<xml_diff>
--- a/Dissertation_ToC_timeline.xlsx
+++ b/Dissertation_ToC_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikbhandari/Documents/docs/phd-and-sfb/academic-writing/papers_abstracts_dissertation/00_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F253B0D0-4D2D-0E4F-B5AA-71C08F3E4320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22E32B3-93C0-3643-BE7A-7C09DE3F358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Chapters</t>
   </si>
@@ -148,9 +148,6 @@
     <t xml:space="preserve">  Procedure</t>
   </si>
   <si>
-    <t xml:space="preserve">  Results and Conclusion</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Conclusion</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Speech processing [Noise vocoding; Speech compression]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Results</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +252,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -355,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,6 +431,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -647,13 +684,14 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="82.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -661,7 +699,7 @@
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -681,7 +719,7 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="10">
         <v>44322</v>
       </c>
@@ -699,7 +737,7 @@
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="12">
         <v>44319</v>
       </c>
@@ -717,7 +755,7 @@
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="14">
         <v>44238</v>
       </c>
@@ -767,7 +805,7 @@
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="28">
         <v>44327</v>
       </c>
@@ -785,7 +823,7 @@
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="16">
         <v>44220</v>
       </c>
@@ -804,7 +842,7 @@
       <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="16">
         <v>44220</v>
       </c>
@@ -821,7 +859,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
@@ -844,7 +882,7 @@
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="14">
         <v>44529</v>
       </c>
@@ -862,7 +900,7 @@
       <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="15">
         <v>44231</v>
       </c>
@@ -880,7 +918,7 @@
       <c r="B13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="14">
         <v>44227</v>
       </c>
@@ -899,7 +937,7 @@
       <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="19">
         <v>44228</v>
       </c>
@@ -918,7 +956,7 @@
       <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="19">
         <v>44229</v>
       </c>
@@ -937,7 +975,7 @@
       <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="15">
         <v>44231</v>
       </c>
@@ -996,7 +1034,7 @@
       <c r="B19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="19">
         <v>44216</v>
       </c>
@@ -1014,7 +1052,7 @@
       <c r="B20" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="19">
         <v>44545</v>
       </c>
@@ -1026,77 +1064,81 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21" s="29">
         <v>6.1</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="15">
+      <c r="C21" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="31">
         <v>44538</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="29">
         <v>7</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22" s="29">
         <v>6.2</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="14">
+      <c r="C22" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="33">
         <v>44540</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="29">
         <v>8</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
+      <c r="A23" s="29">
         <v>6.3</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="31">
+        <v>44545</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="29">
+        <v>9</v>
+      </c>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>6.5</v>
+      </c>
+      <c r="B24" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="15">
+      <c r="C24" s="38"/>
+      <c r="D24" s="35">
         <v>44545</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E24" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="5">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="16">
-        <v>44545</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="F24" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1105,9 +1147,9 @@
         <v>7</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="C25" s="37"/>
       <c r="D25" s="10">
         <v>44283</v>
       </c>
@@ -1123,9 +1165,9 @@
         <v>8</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="C26" s="37"/>
       <c r="D26" s="25">
         <v>44314</v>
       </c>
@@ -1141,9 +1183,9 @@
         <v>9</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="C27" s="37"/>
       <c r="D27" s="19">
         <v>44252</v>
       </c>
@@ -1159,9 +1201,9 @@
         <v>9.1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="C28" s="37"/>
       <c r="D28" s="19">
         <v>44245</v>
       </c>
@@ -1177,9 +1219,9 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="C29" s="37"/>
       <c r="D29" s="19">
         <v>44243</v>
       </c>
@@ -1196,9 +1238,9 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="C30" s="37"/>
       <c r="D30" s="16">
         <v>44248</v>
       </c>
@@ -1214,9 +1256,9 @@
         <v>9.4</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="C31" s="37"/>
       <c r="D31" s="16">
         <v>44250</v>
       </c>
@@ -1232,9 +1274,9 @@
         <v>10</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="C32" s="37"/>
       <c r="D32" s="10">
         <v>44333</v>
       </c>
@@ -1252,7 +1294,7 @@
       <c r="B33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="19">
         <v>44238</v>
       </c>
@@ -1290,7 +1332,7 @@
       <c r="B35" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="19">
         <v>44224</v>
       </c>

</xml_diff>

<commit_message>
Builds up Chapter 6 & Starts Chapter 5 - Almost completes Chapter 6, graded prediction paper - Starts Chapter 5, attentionPrediction manuscript - Renders index.Rmd to main.pdf
</commit_message>
<xml_diff>
--- a/Dissertation_ToC_timeline.xlsx
+++ b/Dissertation_ToC_timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikbhandari/Documents/docs/phd-and-sfb/academic-writing/papers_abstracts_dissertation/00_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22E32B3-93C0-3643-BE7A-7C09DE3F358E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E220A64-2A08-754D-9BB2-A50C70CB191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Chapters</t>
   </si>
@@ -241,7 +241,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -462,6 +468,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -817,39 +855,39 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="40">
         <v>2</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="16">
+      <c r="C8" s="42"/>
+      <c r="D8" s="50">
         <v>44220</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="43">
         <v>11</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="43">
         <v>2.1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="16">
+      <c r="C9" s="42"/>
+      <c r="D9" s="50">
         <v>44220</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="43">
         <v>11</v>
       </c>
       <c r="G9" s="3"/>
@@ -912,20 +950,20 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="43">
         <v>3.1</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="14">
+      <c r="C13" s="42"/>
+      <c r="D13" s="45">
         <v>44227</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="43">
         <v>13</v>
       </c>
       <c r="G13" s="3"/>
@@ -1028,20 +1066,20 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="A19" s="40">
         <v>5</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="19">
+      <c r="C19" s="42"/>
+      <c r="D19" s="48">
         <v>44216</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="43">
         <v>10</v>
       </c>
     </row>
@@ -1112,7 +1150,9 @@
       <c r="B23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="38" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="31">
         <v>44545</v>
       </c>
@@ -1326,20 +1366,20 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="19">
+      <c r="C35" s="42"/>
+      <c r="D35" s="48">
         <v>44224</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="43">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Builds up Chapter 5 & edits 6 - Almost completes Chapter 5 - Edits section titles and other minor edits in Chapter 6
</commit_message>
<xml_diff>
--- a/Dissertation_ToC_timeline.xlsx
+++ b/Dissertation_ToC_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikbhandari/Documents/docs/phd-and-sfb/academic-writing/papers_abstracts_dissertation/00_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E220A64-2A08-754D-9BB2-A50C70CB191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A104639D-84CE-8B41-A2C1-861FBECE0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Chapters</t>
   </si>
@@ -241,7 +241,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +264,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -367,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -436,9 +442,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,12 +456,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -496,10 +493,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -722,14 +737,14 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="82.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="39"/>
+    <col min="3" max="3" width="14.5" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -751,489 +766,501 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="10">
-        <v>44322</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="12">
-        <v>44319</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="5">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>1.2</v>
+      <c r="A4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="37"/>
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" s="14">
-        <v>44238</v>
+        <v>44519</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5">
-        <v>17</v>
+      <c r="F4" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>1.3</v>
+      <c r="A5" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="15">
+        <v>44522</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>1.4</v>
+      <c r="A6" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="D6" s="48">
+        <v>44524</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="28">
-        <v>44327</v>
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="48">
+        <v>44526</v>
       </c>
       <c r="E7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="16">
+        <v>44529</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="16">
+        <v>44531</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40">
-        <v>2</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="50">
-        <v>44220</v>
-      </c>
-      <c r="E8" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="43">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43">
-        <v>2.1</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="50">
-        <v>44220</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="43">
-        <v>11</v>
+      <c r="F9" s="5">
+        <v>6</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>2.2000000000000002</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="16">
-        <v>44526</v>
+        <v>44531</v>
       </c>
       <c r="E10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5">
         <v>6</v>
       </c>
-      <c r="F10" s="5">
-        <v>4</v>
-      </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="14">
-        <v>44529</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="A11" s="28">
+        <v>6.1</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="32">
+        <v>44538</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="28">
+        <v>6.2</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="30">
+        <v>44540</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="14">
+        <v>44545</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="22">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28">
+        <v>6.3</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="49">
+        <v>44545</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="28">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28">
+        <v>6.5</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="49">
+        <v>44545</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="28">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A16" s="37">
+        <v>5</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="50">
+        <v>44216</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="40">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="37">
+        <v>2</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="42">
+        <v>44220</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="F17" s="40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="45">
+        <v>44220</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="45">
+        <v>44224</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="40">
+        <v>3.1</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="45">
+        <v>44227</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="15">
+        <v>44228</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5">
+        <v>14</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="14">
+        <v>44229</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="5">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="15">
+      <c r="C23" s="34"/>
+      <c r="D23" s="15">
         <v>44231</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F23" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="43">
-        <v>3.1</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="45">
-        <v>44227</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="43">
-        <v>13</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="19">
-        <v>44228</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="5">
-        <v>14</v>
-      </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="19">
-        <v>44229</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="5">
-        <v>15</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>3.4</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="15">
+      <c r="C24" s="34"/>
+      <c r="D24" s="16">
         <v>44231</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E24" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F24" s="5">
         <v>16</v>
       </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>4</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="14">
-        <v>44531</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5">
+    </row>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="14">
+        <v>44238</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="19">
-        <v>44531</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A19" s="40">
-        <v>5</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="48">
-        <v>44216</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="43">
+      <c r="F25" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>6</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="19">
-        <v>44545</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="29">
-        <v>6.1</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="31">
-        <v>44538</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="29">
-        <v>7</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="29">
-        <v>6.2</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="33">
-        <v>44540</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="29">
-        <v>8</v>
-      </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="29">
-        <v>6.3</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="31">
-        <v>44545</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="29">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
-        <v>6.5</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="35">
-        <v>44545</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>7</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="10">
-        <v>44283</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>8</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="25">
-        <v>44314</v>
+      <c r="B26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="19">
+        <v>44238</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="5">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>9</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="37"/>
+      <c r="A27" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="34"/>
       <c r="D27" s="19">
-        <v>44252</v>
+        <v>44243</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1243,7 +1270,7 @@
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="19">
         <v>44245</v>
       </c>
@@ -1256,171 +1283,165 @@
     </row>
     <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
-        <v>9.1999999999999993</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="37"/>
+        <v>47</v>
+      </c>
+      <c r="C29" s="34"/>
       <c r="D29" s="19">
-        <v>44243</v>
+        <v>44248</v>
       </c>
       <c r="E29" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="5">
         <v>20</v>
-      </c>
-      <c r="F29" s="5">
-        <v>18</v>
       </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <v>9.3000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="37"/>
+        <v>48</v>
+      </c>
+      <c r="C30" s="34"/>
       <c r="D30" s="16">
-        <v>44248</v>
+        <v>44250</v>
       </c>
       <c r="E30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>9</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="16">
+        <v>44252</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="5">
         <v>22</v>
       </c>
-      <c r="F30" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
-        <v>9.4</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="16">
-        <v>44250</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" ht="38" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
-        <v>10</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="37"/>
+        <v>7</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="34"/>
       <c r="D32" s="10">
-        <v>44333</v>
+        <v>44283</v>
       </c>
       <c r="E32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="38" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
         <v>8</v>
       </c>
-      <c r="F32" s="18">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="19">
-        <v>44238</v>
+      <c r="B33" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="25">
+        <v>44314</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="5">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>15</v>
+      <c r="A34" s="5">
+        <v>1.1000000000000001</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="19">
-        <v>44519</v>
+        <v>7</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="25">
+        <v>44319</v>
       </c>
       <c r="E34" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>1</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="25">
+        <v>44322</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="48">
-        <v>44224</v>
-      </c>
-      <c r="E35" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="43">
-        <v>12</v>
+      <c r="F35" s="5">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>24</v>
+      <c r="A36" s="5">
+        <v>1.5</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="15">
-        <v>44522</v>
+        <v>19</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="12">
+        <v>44327</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F36" s="5">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="16">
-        <v>44524</v>
+      <c r="A37" s="7">
+        <v>10</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="51">
+        <v>44333</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="5">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="F37" s="18">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7204,7 +7225,7 @@
   </sheetData>
   <autoFilter ref="A1:F37" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
-      <sortCondition ref="A1:A37"/>
+      <sortCondition ref="F1:F37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Splits contents within Chapter 7 - Changes the chapter contents from within group design to Two experiments Chapter - Minor editorial changes in chapter 5 and 6 - Adds notes in the ToC after last week's supervision meeting
</commit_message>
<xml_diff>
--- a/Dissertation_ToC_timeline.xlsx
+++ b/Dissertation_ToC_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikbhandari/Documents/docs/phd-and-sfb/academic-writing/papers_abstracts_dissertation/00_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A104639D-84CE-8B41-A2C1-861FBECE0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FF5A16-E806-674B-B7CD-DBA0A4818BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Chapters</t>
   </si>
@@ -738,7 +738,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1087,7 +1087,9 @@
       <c r="B18" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="40" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="45">
         <v>44220</v>
       </c>
@@ -1234,7 +1236,9 @@
       <c r="B26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="40" t="s">
+        <v>13</v>
+      </c>
       <c r="D26" s="19">
         <v>44238</v>
       </c>

</xml_diff>

<commit_message>
Formats Chaptering @ 1,2,3 - Changes chapters 1,2, & 3 to Intro, Background and Methods - Collapses previous chapter 2 and 3 into chapter 3 - Creates new chapter Background as chapter 2 - Inspired from Merel's thesis and JK/VD's comments - Adds structure of new format in ToC.doc file
</commit_message>
<xml_diff>
--- a/Dissertation_ToC_timeline.xlsx
+++ b/Dissertation_ToC_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikbhandari/Documents/docs/phd-and-sfb/academic-writing/papers_abstracts_dissertation/00_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FF5A16-E806-674B-B7CD-DBA0A4818BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED8E41B-3A79-0C43-91F8-14CEFA515D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6560" yWindow="-24300" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,28 +493,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -766,505 +760,497 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="10">
+        <v>44322</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="12">
+        <v>44319</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="5">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
+      <c r="A4" s="5">
+        <v>1.2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C4" s="34"/>
       <c r="D4" s="14">
-        <v>44519</v>
+        <v>44238</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="18">
-        <v>1</v>
+      <c r="F4" s="5">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>24</v>
+      <c r="A5" s="5">
+        <v>1.3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="15">
-        <v>44522</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>22</v>
-      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>26</v>
+      <c r="A6" s="5">
+        <v>1.4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48">
-        <v>44524</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>20</v>
-      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="50">
+        <v>44327</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="37">
+        <v>2</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="49">
+        <v>44220</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="40">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="48">
-        <v>44526</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="16">
-        <v>44529</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="D9" s="49">
+        <v>44220</v>
+      </c>
+      <c r="E9" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="5">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="16">
-        <v>44531</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="5">
-        <v>6</v>
+      <c r="F9" s="40">
+        <v>11</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>4.0999999999999996</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="16">
+        <v>44526</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="14">
+        <v>44529</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="15">
+        <v>44231</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3.1</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="42">
+        <v>44227</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="40">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="19">
+        <v>44228</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5">
+        <v>14</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="19">
+        <v>44229</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="5">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="15">
+        <v>44231</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5">
+        <v>16</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="14">
         <v>44531</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F17" s="5">
         <v>6</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="19">
+        <v>44531</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A19" s="37">
+        <v>5</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="45">
+        <v>44216</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>6</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="19">
+        <v>44545</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="28">
         <v>6.1</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B21" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C21" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D21" s="30">
         <v>44538</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F21" s="28">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="28">
         <v>6.2</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B22" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C22" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D22" s="32">
         <v>44540</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E22" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F22" s="28">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>6</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="28">
+        <v>6.3</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D23" s="30">
         <v>44545</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E23" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F23" s="28">
         <v>9</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
-        <v>6.3</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="35" t="s">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="28">
+        <v>6.5</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="49">
+      <c r="D24" s="48">
         <v>44545</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E24" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F24" s="28">
         <v>9</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28">
-        <v>6.5</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="49">
-        <v>44545</v>
-      </c>
-      <c r="E15" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="28">
-        <v>9</v>
-      </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="38" x14ac:dyDescent="0.2">
-      <c r="A16" s="37">
-        <v>5</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="50">
-        <v>44216</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="40">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="37">
-        <v>2</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="42">
-        <v>44220</v>
-      </c>
-      <c r="E17" s="43" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>7</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="10">
+        <v>44283</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="40">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="B18" s="44" t="s">
+      <c r="F25" s="5">
         <v>23</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="45">
-        <v>44220</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="40">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="45">
-        <v>44224</v>
-      </c>
-      <c r="E19" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="40">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="40">
-        <v>3.1</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="45">
-        <v>44227</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="40">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="15">
-        <v>44228</v>
-      </c>
-      <c r="E21" s="13" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
         <v>8</v>
       </c>
-      <c r="F21" s="5">
-        <v>14</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="14">
-        <v>44229</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="5">
-        <v>15</v>
-      </c>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>3</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="15">
-        <v>44231</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="5">
-        <v>16</v>
-      </c>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="16">
-        <v>44231</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="14">
-        <v>44238</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="19">
-        <v>44238</v>
+      <c r="B26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="25">
+        <v>44314</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="5">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>46</v>
+      <c r="A27" s="7">
+        <v>9</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="C27" s="34"/>
       <c r="D27" s="19">
-        <v>44243</v>
+        <v>44252</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F27" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1287,165 +1273,173 @@
     </row>
     <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
-        <v>9.3000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="34"/>
       <c r="D29" s="19">
-        <v>44248</v>
+        <v>44243</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F29" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <v>9.4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="34"/>
       <c r="D30" s="16">
-        <v>44250</v>
+        <v>44248</v>
       </c>
       <c r="E30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="5">
         <v>20</v>
       </c>
-      <c r="F30" s="5">
-        <v>21</v>
-      </c>
     </row>
     <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>9</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>44</v>
+      <c r="A31" s="5">
+        <v>9.4</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="16">
-        <v>44252</v>
+        <v>44250</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F31" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="38" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
-        <v>7</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="10">
-        <v>44283</v>
+        <v>44333</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="38" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
         <v>8</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="25">
-        <v>44314</v>
+      <c r="F32" s="18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="19">
+        <v>44238</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="19">
+        <v>44519</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="45">
+        <v>44224</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="25">
-        <v>44319</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="5">
+      <c r="B36" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>1</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="25">
-        <v>44322</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="5">
+      <c r="C36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="15">
+        <v>44522</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="12">
-        <v>44327</v>
-      </c>
-      <c r="E36" s="13" t="s">
+      <c r="B37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="16">
+        <v>44524</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>10</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="51">
-        <v>44333</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="18">
-        <v>28</v>
+      <c r="F37" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7229,7 +7223,7 @@
   </sheetData>
   <autoFilter ref="A1:F37" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
-      <sortCondition ref="F1:F37"/>
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>